<commit_message>
Updates Chapter 4 main text and Table 4.1
</commit_message>
<xml_diff>
--- a/4_Evolution_of_retinol_metabolism/Table_4.1_kegg_components/Table_4.1.xlsx
+++ b/4_Evolution_of_retinol_metabolism/Table_4.1_kegg_components/Table_4.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING_Clone_current/4_Evolution_of_retinol_metabolism/Table_4.1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING_Clone_current/4_Evolution_of_retinol_metabolism/Table_4.1_kegg_components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{236ADE17-AAB9-436F-BEF3-31DA2531A3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DF1A925-7A22-4253-9140-CEFD5835C15E}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{236ADE17-AAB9-436F-BEF3-31DA2531A3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE72A024-8F7B-446D-B355-B709D4EF72B9}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5551D420-99A4-4812-AAA2-4416EDA5A17B}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>patatin-like phospholipase domain-containing protein 4</t>
   </si>
   <si>
-    <t># Pathways</t>
-  </si>
-  <si>
     <t xml:space="preserve">K09516 </t>
   </si>
   <si>
@@ -534,6 +531,9 @@
   </si>
   <si>
     <t>Retinol Metabolism</t>
+  </si>
+  <si>
+    <t>Num Kegg Pathways</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -597,21 +597,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -772,21 +757,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -826,6 +796,17 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -835,7 +816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -847,86 +828,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -943,6 +930,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1245,7 +1236,7 @@
   <dimension ref="B1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1260,71 +1251,71 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="2:6" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="28"/>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="33"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="22" t="s">
+      <c r="D5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="20">
+      <c r="F5" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:6" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="F6" s="17">
+        <v>161</v>
+      </c>
+      <c r="F6" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1341,734 +1332,734 @@
       <c r="E7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="27"/>
+      <c r="C9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="27"/>
+      <c r="C10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="18">
+      <c r="D10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="11"/>
-      <c r="C9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="13" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="27"/>
+      <c r="C11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="27"/>
+      <c r="C12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="19">
+      <c r="D12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="17">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="13" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="28"/>
+      <c r="C13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
-      <c r="C13" s="15" t="s">
+      <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="20">
+      <c r="F13" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="17">
+      <c r="F14" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="17">
+      <c r="F15" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="17">
+      <c r="F16" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="17">
+      <c r="F17" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="27"/>
+      <c r="C19" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="27"/>
+      <c r="C20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="27"/>
+      <c r="C21" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="27"/>
+      <c r="C22" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="42" x14ac:dyDescent="0.35">
+      <c r="B23" s="28"/>
+      <c r="C23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="28"/>
+      <c r="C25" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="18">
+      <c r="C26" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="27"/>
+      <c r="C27" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="11"/>
-      <c r="C19" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="19">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="27"/>
+      <c r="C28" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="11"/>
-      <c r="C20" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="19">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="27"/>
+      <c r="C29" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="27"/>
+      <c r="C30" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="27"/>
+      <c r="C31" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="27"/>
+      <c r="C32" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="17">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="11"/>
-      <c r="C21" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="11"/>
-      <c r="C22" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="B23" s="14"/>
-      <c r="C23" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="20">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B33" s="27"/>
+      <c r="C33" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" s="17">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="10" t="s">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B34" s="27"/>
+      <c r="C34" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B35" s="27"/>
+      <c r="C35" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B36" s="27"/>
+      <c r="C36" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="27"/>
+      <c r="C37" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B38" s="27"/>
+      <c r="C38" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B39" s="27"/>
+      <c r="C39" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B40" s="27"/>
+      <c r="C40" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B41" s="27"/>
+      <c r="C41" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="27"/>
+      <c r="C42" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B43" s="27"/>
+      <c r="C43" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" s="17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B44" s="27"/>
+      <c r="C44" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="14"/>
-      <c r="C25" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F26" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="11"/>
-      <c r="C28" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" s="13" t="s">
+      <c r="D44" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B45" s="27"/>
+      <c r="C45" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F28" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="11"/>
-      <c r="C29" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="11"/>
-      <c r="C30" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="11"/>
-      <c r="C31" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B32" s="11"/>
-      <c r="C32" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="F32" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B33" s="11"/>
-      <c r="C33" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="F33" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B34" s="11"/>
-      <c r="C34" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B35" s="11"/>
-      <c r="C35" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="F35" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B36" s="11"/>
-      <c r="C36" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="F36" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B37" s="11"/>
-      <c r="C37" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="F37" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B38" s="11"/>
-      <c r="C38" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="F38" s="19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B39" s="11"/>
-      <c r="C39" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B40" s="11"/>
-      <c r="C40" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="F40" s="19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B41" s="11"/>
-      <c r="C41" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F41" s="19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B42" s="11"/>
-      <c r="C42" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F42" s="19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B43" s="11"/>
-      <c r="C43" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F43" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B44" s="11"/>
-      <c r="C44" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" s="13" t="s">
+      <c r="D45" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F45" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="28"/>
+      <c r="C46" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F44" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B45" s="11"/>
-      <c r="C45" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="F45" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B46" s="14"/>
-      <c r="C46" s="15" t="s">
+      <c r="D46" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="E46" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E46" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F46" s="20">
+      <c r="F46" s="18">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B47" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E47" s="7" t="s">
+      <c r="F47" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B48" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F48" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B49" s="27"/>
+      <c r="C49" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="F47" s="17">
+      <c r="D49" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F49" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B48" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E48" s="10" t="s">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B50" s="27"/>
+      <c r="C50" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F48" s="18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B49" s="11"/>
-      <c r="C49" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="F49" s="19">
+      <c r="D50" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F50" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B50" s="11"/>
-      <c r="C50" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E50" s="13" t="s">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B51" s="27"/>
+      <c r="C51" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F51" s="17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B52" s="27"/>
+      <c r="C52" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="F50" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B51" s="11"/>
-      <c r="C51" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="D51" s="12" t="s">
+      <c r="D52" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="F52" s="17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="B53" s="28"/>
+      <c r="C53" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E51" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="F51" s="19">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B52" s="11"/>
-      <c r="C52" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F52" s="19">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="B53" s="14"/>
-      <c r="C53" s="15" t="s">
+      <c r="D53" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="E53" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="E53" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="F53" s="20">
+      <c r="F53" s="18">
         <v>16</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B54" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C54" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F54" s="17">
+      <c r="F54" s="15">
         <v>14</v>
       </c>
     </row>
@@ -2077,15 +2068,16 @@
     <sortCondition ref="F48:F53"/>
     <sortCondition ref="C48:C53"/>
   </sortState>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B26:B46"/>
+    <mergeCell ref="B48:B53"/>
+    <mergeCell ref="C3:E3"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B18:B23"/>
-    <mergeCell ref="B26:B46"/>
-    <mergeCell ref="B48:B53"/>
-    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates all Figs and notes in manuscript Chapter 4
</commit_message>
<xml_diff>
--- a/4_Evolution_of_retinol_metabolism/Table_4.1_kegg_components/Table_4.1.xlsx
+++ b/4_Evolution_of_retinol_metabolism/Table_4.1_kegg_components/Table_4.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING_Clone_current/4_Evolution_of_retinol_metabolism/Table_4.1_kegg_components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{236ADE17-AAB9-436F-BEF3-31DA2531A3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE72A024-8F7B-446D-B355-B709D4EF72B9}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{236ADE17-AAB9-436F-BEF3-31DA2531A3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB6968B1-9E6F-45F4-874F-E56F3D3D03C2}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5551D420-99A4-4812-AAA2-4416EDA5A17B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="165">
   <si>
     <t>Entry</t>
   </si>
@@ -506,15 +506,9 @@
     <t>BCMO1</t>
   </si>
   <si>
-    <t>CCO</t>
-  </si>
-  <si>
     <t>DGAT</t>
   </si>
   <si>
-    <t>SDR</t>
-  </si>
-  <si>
     <t>CYP</t>
   </si>
   <si>
@@ -534,6 +528,9 @@
   </si>
   <si>
     <t>Num Kegg Pathways</t>
+  </si>
+  <si>
+    <t>DHRS</t>
   </si>
 </sst>
 </file>
@@ -876,6 +873,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -890,24 +905,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1236,7 +1233,7 @@
   <dimension ref="B1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1251,29 +1248,29 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
+      <c r="B2" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="32" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="4" spans="2:6" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="25"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="19" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1310,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F6" s="15">
         <v>1</v>
@@ -1337,7 +1334,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="21" t="s">
         <v>153</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -1354,7 +1351,7 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="27"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="10" t="s">
         <v>20</v>
       </c>
@@ -1369,7 +1366,7 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="27"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="10" t="s">
         <v>17</v>
       </c>
@@ -1384,7 +1381,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="27"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="10" t="s">
         <v>11</v>
       </c>
@@ -1399,7 +1396,7 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="27"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="10" t="s">
         <v>23</v>
       </c>
@@ -1414,7 +1411,7 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="28"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="13" t="s">
         <v>26</v>
       </c>
@@ -1447,7 +1444,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>38</v>
@@ -1497,8 +1494,8 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="26" t="s">
-        <v>158</v>
+      <c r="B18" s="21" t="s">
+        <v>164</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>44</v>
@@ -1514,7 +1511,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="27"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="10" t="s">
         <v>50</v>
       </c>
@@ -1529,7 +1526,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="27"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="10" t="s">
         <v>47</v>
       </c>
@@ -1544,7 +1541,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="27"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="10" t="s">
         <v>41</v>
       </c>
@@ -1559,7 +1556,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="27"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="10" t="s">
         <v>53</v>
       </c>
@@ -1574,7 +1571,7 @@
       </c>
     </row>
     <row r="23" spans="2:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="B23" s="28"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="13" t="s">
         <v>56</v>
       </c>
@@ -1589,8 +1586,8 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="26" t="s">
-        <v>157</v>
+      <c r="B24" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>62</v>
@@ -1606,7 +1603,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="28"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="13" t="s">
         <v>59</v>
       </c>
@@ -1621,8 +1618,8 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="26" t="s">
-        <v>159</v>
+      <c r="B26" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>128</v>
@@ -1638,7 +1635,7 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="27"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="10" t="s">
         <v>74</v>
       </c>
@@ -1653,7 +1650,7 @@
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="27"/>
+      <c r="B28" s="22"/>
       <c r="C28" s="10" t="s">
         <v>107</v>
       </c>
@@ -1668,7 +1665,7 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="27"/>
+      <c r="B29" s="22"/>
       <c r="C29" s="10" t="s">
         <v>98</v>
       </c>
@@ -1683,7 +1680,7 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="27"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="10" t="s">
         <v>101</v>
       </c>
@@ -1698,7 +1695,7 @@
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="27"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="10" t="s">
         <v>104</v>
       </c>
@@ -1713,7 +1710,7 @@
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B32" s="27"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="10" t="s">
         <v>95</v>
       </c>
@@ -1728,7 +1725,7 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B33" s="27"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="10" t="s">
         <v>116</v>
       </c>
@@ -1743,7 +1740,7 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B34" s="27"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="10" t="s">
         <v>89</v>
       </c>
@@ -1758,7 +1755,7 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B35" s="27"/>
+      <c r="B35" s="22"/>
       <c r="C35" s="10" t="s">
         <v>80</v>
       </c>
@@ -1773,7 +1770,7 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B36" s="27"/>
+      <c r="B36" s="22"/>
       <c r="C36" s="10" t="s">
         <v>119</v>
       </c>
@@ -1788,7 +1785,7 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B37" s="27"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="10" t="s">
         <v>113</v>
       </c>
@@ -1803,7 +1800,7 @@
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B38" s="27"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="10" t="s">
         <v>122</v>
       </c>
@@ -1818,7 +1815,7 @@
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B39" s="27"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="10" t="s">
         <v>77</v>
       </c>
@@ -1833,7 +1830,7 @@
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B40" s="27"/>
+      <c r="B40" s="22"/>
       <c r="C40" s="10" t="s">
         <v>92</v>
       </c>
@@ -1848,7 +1845,7 @@
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B41" s="27"/>
+      <c r="B41" s="22"/>
       <c r="C41" s="10" t="s">
         <v>71</v>
       </c>
@@ -1863,7 +1860,7 @@
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B42" s="27"/>
+      <c r="B42" s="22"/>
       <c r="C42" s="10" t="s">
         <v>83</v>
       </c>
@@ -1878,7 +1875,7 @@
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B43" s="27"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="10" t="s">
         <v>86</v>
       </c>
@@ -1893,7 +1890,7 @@
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B44" s="27"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="10" t="s">
         <v>65</v>
       </c>
@@ -1908,7 +1905,7 @@
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B45" s="27"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="10" t="s">
         <v>110</v>
       </c>
@@ -1923,7 +1920,7 @@
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B46" s="28"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="13" t="s">
         <v>68</v>
       </c>
@@ -1955,8 +1952,8 @@
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B48" s="26" t="s">
-        <v>160</v>
+      <c r="B48" s="21" t="s">
+        <v>158</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>137</v>
@@ -1972,7 +1969,7 @@
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B49" s="27"/>
+      <c r="B49" s="22"/>
       <c r="C49" s="10" t="s">
         <v>134</v>
       </c>
@@ -1987,7 +1984,7 @@
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B50" s="27"/>
+      <c r="B50" s="22"/>
       <c r="C50" s="10" t="s">
         <v>140</v>
       </c>
@@ -2002,7 +1999,7 @@
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B51" s="27"/>
+      <c r="B51" s="22"/>
       <c r="C51" s="10" t="s">
         <v>146</v>
       </c>
@@ -2017,7 +2014,7 @@
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B52" s="27"/>
+      <c r="B52" s="22"/>
       <c r="C52" s="10" t="s">
         <v>143</v>
       </c>
@@ -2032,7 +2029,7 @@
       </c>
     </row>
     <row r="53" spans="2:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="B53" s="28"/>
+      <c r="B53" s="23"/>
       <c r="C53" s="13" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
Writing Chapter 4 and small Figure edits
</commit_message>
<xml_diff>
--- a/4_Evolution_of_retinol_metabolism/Table_4.1_kegg_components/Table_4.1.xlsx
+++ b/4_Evolution_of_retinol_metabolism/Table_4.1_kegg_components/Table_4.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING_Clone_current/4_Evolution_of_retinol_metabolism/Table_4.1_kegg_components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{236ADE17-AAB9-436F-BEF3-31DA2531A3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB6968B1-9E6F-45F4-874F-E56F3D3D03C2}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{236ADE17-AAB9-436F-BEF3-31DA2531A3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{622CBA24-269B-4185-9C8B-DB4187432DF7}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5551D420-99A4-4812-AAA2-4416EDA5A17B}"/>
   </bookViews>
@@ -200,9 +200,6 @@
     <t>K15734</t>
   </si>
   <si>
-    <t>SDR16C5</t>
-  </si>
-  <si>
     <t>all-trans-retinol dehydrogenase (NAD+)</t>
   </si>
   <si>
@@ -531,6 +528,9 @@
   </si>
   <si>
     <t>DHRS</t>
+  </si>
+  <si>
+    <t>SDR16C5 (RDHE2)</t>
   </si>
 </sst>
 </file>
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF95D34F-DFC4-4168-9B49-08F8919867C4}">
   <dimension ref="B1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1249,7 +1249,7 @@
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="B2" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
@@ -1258,15 +1258,15 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>160</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>161</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="26"/>
       <c r="F3" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="2:6" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1301,7 +1301,7 @@
     </row>
     <row r="6" spans="2:6" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>9</v>
@@ -1310,7 +1310,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F6" s="15">
         <v>1</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>14</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>29</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>35</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>44</v>
@@ -1561,10 +1561,10 @@
         <v>53</v>
       </c>
       <c r="D22" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="F22" s="17">
         <v>3</v>
@@ -1573,13 +1573,13 @@
     <row r="23" spans="2:6" ht="42" x14ac:dyDescent="0.35">
       <c r="B23" s="23"/>
       <c r="C23" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="E23" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>58</v>
       </c>
       <c r="F23" s="18">
         <v>4</v>
@@ -1587,16 +1587,16 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="E24" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="F24" s="16">
         <v>3</v>
@@ -1605,13 +1605,13 @@
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="23"/>
       <c r="C25" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="E25" s="14" t="s">
         <v>60</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>61</v>
       </c>
       <c r="F25" s="18">
         <v>4</v>
@@ -1619,16 +1619,16 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C26" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E26" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="F26" s="16">
         <v>1</v>
@@ -1637,13 +1637,13 @@
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="22"/>
       <c r="C27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="E27" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="F27" s="17">
         <v>2</v>
@@ -1652,13 +1652,13 @@
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="22"/>
       <c r="C28" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="F28" s="17">
         <v>2</v>
@@ -1667,13 +1667,13 @@
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="22"/>
       <c r="C29" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="E29" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>100</v>
       </c>
       <c r="F29" s="17">
         <v>2</v>
@@ -1682,13 +1682,13 @@
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="22"/>
       <c r="C30" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>103</v>
       </c>
       <c r="F30" s="17">
         <v>2</v>
@@ -1697,13 +1697,13 @@
     <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" s="22"/>
       <c r="C31" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="E31" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>106</v>
       </c>
       <c r="F31" s="17">
         <v>2</v>
@@ -1712,13 +1712,13 @@
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B32" s="22"/>
       <c r="C32" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="F32" s="17">
         <v>3</v>
@@ -1727,13 +1727,13 @@
     <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B33" s="22"/>
       <c r="C33" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="F33" s="17">
         <v>4</v>
@@ -1742,13 +1742,13 @@
     <row r="34" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B34" s="22"/>
       <c r="C34" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>91</v>
       </c>
       <c r="F34" s="17">
         <v>4</v>
@@ -1757,13 +1757,13 @@
     <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B35" s="22"/>
       <c r="C35" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="E35" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>82</v>
       </c>
       <c r="F35" s="17">
         <v>5</v>
@@ -1772,13 +1772,13 @@
     <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36" s="22"/>
       <c r="C36" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="E36" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="F36" s="17">
         <v>6</v>
@@ -1787,13 +1787,13 @@
     <row r="37" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B37" s="22"/>
       <c r="C37" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="E37" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>115</v>
       </c>
       <c r="F37" s="17">
         <v>6</v>
@@ -1802,13 +1802,13 @@
     <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" s="22"/>
       <c r="C38" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>124</v>
       </c>
       <c r="F38" s="17">
         <v>7</v>
@@ -1817,13 +1817,13 @@
     <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39" s="22"/>
       <c r="C39" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="E39" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>79</v>
       </c>
       <c r="F39" s="17">
         <v>7</v>
@@ -1832,13 +1832,13 @@
     <row r="40" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B40" s="22"/>
       <c r="C40" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="11" t="s">
         <v>93</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>94</v>
       </c>
       <c r="F40" s="17">
         <v>8</v>
@@ -1847,13 +1847,13 @@
     <row r="41" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B41" s="22"/>
       <c r="C41" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="E41" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="F41" s="17">
         <v>8</v>
@@ -1862,13 +1862,13 @@
     <row r="42" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B42" s="22"/>
       <c r="C42" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>85</v>
       </c>
       <c r="F42" s="17">
         <v>8</v>
@@ -1877,13 +1877,13 @@
     <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B43" s="22"/>
       <c r="C43" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="E43" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="F43" s="17">
         <v>9</v>
@@ -1892,13 +1892,13 @@
     <row r="44" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B44" s="22"/>
       <c r="C44" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="F44" s="17">
         <v>10</v>
@@ -1907,13 +1907,13 @@
     <row r="45" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B45" s="22"/>
       <c r="C45" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="E45" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="F45" s="17">
         <v>10</v>
@@ -1922,13 +1922,13 @@
     <row r="46" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B46" s="23"/>
       <c r="C46" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="E46" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>70</v>
       </c>
       <c r="F46" s="18">
         <v>12</v>
@@ -1936,16 +1936,16 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B47" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="F47" s="15">
         <v>10</v>
@@ -1953,16 +1953,16 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B48" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C48" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="E48" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>139</v>
       </c>
       <c r="F48" s="16">
         <v>9</v>
@@ -1971,13 +1971,13 @@
     <row r="49" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B49" s="22"/>
       <c r="C49" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="E49" s="11" t="s">
         <v>135</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>136</v>
       </c>
       <c r="F49" s="17">
         <v>10</v>
@@ -1986,13 +1986,13 @@
     <row r="50" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B50" s="22"/>
       <c r="C50" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D50" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="E50" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="F50" s="17">
         <v>10</v>
@@ -2001,13 +2001,13 @@
     <row r="51" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B51" s="22"/>
       <c r="C51" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51" s="11" t="s">
         <v>146</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="F51" s="17">
         <v>13</v>
@@ -2016,13 +2016,13 @@
     <row r="52" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B52" s="22"/>
       <c r="C52" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="E52" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>145</v>
       </c>
       <c r="F52" s="17">
         <v>13</v>
@@ -2031,13 +2031,13 @@
     <row r="53" spans="2:6" ht="28" x14ac:dyDescent="0.35">
       <c r="B53" s="23"/>
       <c r="C53" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="E53" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F53" s="18">
         <v>16</v>
@@ -2045,16 +2045,16 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B54" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="F54" s="15">
         <v>14</v>

</xml_diff>